<commit_message>
Added billing details code
</commit_message>
<xml_diff>
--- a/src/test/resources/commonData.xlsx
+++ b/src/test/resources/commonData.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28526"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SPidugujothi\IdeaProjects\Data_Extract\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24A5CD7D-C99D-462D-8690-8175DDCFC2B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02813D59-6F12-46EB-A27C-4A7F9266101B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t>URL</t>
   </si>
@@ -61,6 +61,12 @@
   </si>
   <si>
     <t>edge</t>
+  </si>
+  <si>
+    <t>Application name</t>
+  </si>
+  <si>
+    <t>demowebshop</t>
   </si>
 </sst>
 </file>
@@ -418,10 +424,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E3"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -431,9 +437,10 @@
     <col min="3" max="3" width="21.44140625" customWidth="1"/>
     <col min="4" max="4" width="12.33203125" customWidth="1"/>
     <col min="5" max="5" width="8.88671875" style="8"/>
+    <col min="6" max="6" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A1" s="4" t="s">
         <v>8</v>
       </c>
@@ -449,8 +456,11 @@
       <c r="E1" s="6" t="s">
         <v>6</v>
       </c>
+      <c r="F1" s="1" t="s">
+        <v>12</v>
+      </c>
     </row>
-    <row r="2" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A2" s="4">
         <v>1</v>
       </c>
@@ -466,8 +476,11 @@
       <c r="E2" s="7" t="s">
         <v>7</v>
       </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
     </row>
-    <row r="3" spans="1:5" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:6" ht="28.8" x14ac:dyDescent="0.3">
       <c r="A3" s="4">
         <v>2</v>
       </c>

</xml_diff>